<commit_message>
Added and improved working with Name(s) for Application, Workbook, Worksheet, and Range.
</commit_message>
<xml_diff>
--- a/samples/XLSpy/sample.xlsx
+++ b/samples/XLSpy/sample.xlsx
@@ -14,6 +14,9 @@
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="Numbers">'a worksheet'!$A$2:$A$6</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -217,7 +220,7 @@
             <c:numRef>
               <c:f>'a worksheet'!$A$2:$A$6</c:f>
               <c:numCache>
-                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
@@ -247,11 +250,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="156224512"/>
-        <c:axId val="113316608"/>
+        <c:axId val="225302400"/>
+        <c:axId val="225303936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156224512"/>
+        <c:axId val="225302400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -260,7 +263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113316608"/>
+        <c:crossAx val="225303936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -268,18 +271,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113316608"/>
+        <c:axId val="225303936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Vęeobecný" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156224512"/>
+        <c:crossAx val="225302400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -344,7 +347,7 @@
             <c:numRef>
               <c:f>'a worksheet'!$A$2:$A$6</c:f>
               <c:numCache>
-                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
@@ -374,11 +377,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="114362240"/>
-        <c:axId val="114363776"/>
+        <c:axId val="207197312"/>
+        <c:axId val="207198848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114362240"/>
+        <c:axId val="207197312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114363776"/>
+        <c:crossAx val="207198848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -395,18 +398,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114363776"/>
+        <c:axId val="207198848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="Vęeobecný" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114362240"/>
+        <c:crossAx val="207197312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -661,7 +664,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Calibri"/>
-                  <a:cs typeface="Calibri"/>
                 </a:rPr>
                 <a:t>Button</a:t>
               </a:r>
@@ -1137,7 +1139,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add support for tables
Add support for Excel tables (formerly known as Excel lists).
</commit_message>
<xml_diff>
--- a/samples/XLSpy/sample.xlsx
+++ b/samples/XLSpy/sample.xlsx
@@ -1,33 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" backupFile="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7C6CB1-9134-4015-87ED-82419A0B1F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="24780" windowHeight="12660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a worksheet" sheetId="1" r:id="rId1"/>
     <sheet name="a chart" sheetId="4" r:id="rId2"/>
+    <sheet name="a list" sheetId="5" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="Numbers">'a worksheet'!$A$2:$A$6</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -38,7 +50,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -53,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +76,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -84,25 +96,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Numbers</t>
   </si>
   <si>
     <t>A hyperlink</t>
   </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>ABC0123</t>
+  </si>
+  <si>
+    <t>XYZ4567</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -121,13 +168,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -135,6 +175,12 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,160 +200,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="7" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+  <cellStyles count="4">
+    <cellStyle name="Currency 2" xfId="3" xr:uid="{FC3B6029-A97E-4655-84B2-C301919B4353}"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{3107779C-F047-481D-B3AC-7B423F6FEF4A}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="cs-CZ"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'a worksheet'!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Numbers</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'a worksheet'!$A$2:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="225302400"/>
-        <c:axId val="225303936"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="225302400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225303936"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="225303936"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225302400"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="cs-CZ"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -367,6 +335,142 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DEA9-4E4C-B194-03C10826F2A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="225302400"/>
+        <c:axId val="225303936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="225302400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="225303936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="225303936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="225302400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'a worksheet'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Numbers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'a worksheet'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6971-4F7E-AE6F-80CC0DB1035F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -426,10 +530,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Graf2"/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -458,7 +562,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graf 1"/>
+        <xdr:cNvPr id="2" name="Graf 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -490,6 +600,11 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Obdélník 2">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -552,7 +667,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Obrázek 3"/>
+        <xdr:cNvPr id="4" name="Obrázek 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -580,15 +701,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>400050</xdr:colOff>
+          <xdr:colOff>403860</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>47625</xdr:colOff>
+          <xdr:colOff>45720</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -597,11 +718,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -609,6 +733,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -621,15 +756,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>295275</xdr:colOff>
+          <xdr:colOff>297180</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>335280</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -638,11 +773,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -650,20 +788,27 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="cs-CZ" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
                 </a:rPr>
                 <a:t>Button</a:t>
               </a:r>
@@ -682,13 +827,13 @@
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
+          <xdr:colOff>60960</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -697,11 +842,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -709,6 +857,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -727,9 +886,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>514350</xdr:colOff>
+          <xdr:colOff>518160</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -738,11 +897,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -750,6 +912,16 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -762,15 +934,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>16</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
+          <xdr:colOff>487680</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -779,11 +951,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -791,6 +966,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -805,10 +991,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9279659" cy="6018068"/>
+    <xdr:ext cx="9285339" cy="5997677"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graf 1"/>
+        <xdr:cNvPr id="2" name="Graf 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -848,10 +1040,24 @@
 </externalLink>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0842BD24-2BB2-4B5B-BA5D-4111B4C2BE75}" name="Table1" displayName="Table1" ref="A1:E4" totalsRowCount="1" headerRowCellStyle="Normal 2">
+  <autoFilter ref="A1:E3" xr:uid="{F259B205-2D84-45D9-B744-3E6B6664A265}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{BC7DE907-5637-4F47-8C37-06279ED14DD5}" name="Code" totalsRowLabel="Total" dataCellStyle="Normal 2" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{42D27FF3-2BB5-4E09-AE05-5A5AE07AB8F4}" name="Date"/>
+    <tableColumn id="3" xr3:uid="{E440527C-9FD7-4563-862A-BEB449ED5DCE}" name="Quantity" dataCellStyle="Normal 2" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{E51F2751-6973-4473-A8CD-8575B17BE611}" name="Price"/>
+    <tableColumn id="5" xr3:uid="{9EF5BB04-06F5-4DBD-971C-9674080F1DD8}" name="Subtotal" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency 2" totalsRowCellStyle="Currency 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -889,9 +1095,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -924,9 +1130,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -959,9 +1182,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1134,57 +1374,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1"/>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="landscape" r:id="rId2"/>
@@ -1198,15 +1438,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>400050</xdr:colOff>
+                <xdr:colOff>403860</xdr:colOff>
                 <xdr:row>15</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:rowOff>106680</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
+                <xdr:colOff>45720</xdr:colOff>
                 <xdr:row>16</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>83820</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1225,13 +1465,13 @@
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>15</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>7620</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>14</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
+                <xdr:colOff>60960</xdr:colOff>
                 <xdr:row>28</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:rowOff>30480</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1254,9 +1494,9 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
+                <xdr:colOff>518160</xdr:colOff>
                 <xdr:row>23</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>175260</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1273,15 +1513,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
+                <xdr:colOff>480060</xdr:colOff>
                 <xdr:row>30</xdr:row>
                 <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>16</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
+                <xdr:colOff>487680</xdr:colOff>
                 <xdr:row>37</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>45720</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1302,15 +1542,15 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>295275</xdr:colOff>
+                    <xdr:colOff>297180</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>333375</xdr:colOff>
+                    <xdr:colOff>335280</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:rowOff>182880</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1321,4 +1561,89 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E8CBAC-CEEF-4BCB-B63E-77124C8DE438}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44021</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="E2" s="5">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44021</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8.25</v>
+      </c>
+      <c r="E3" s="5">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="E4" s="7">
+        <f>SUBTOTAL(109,Table1[Subtotal])</f>
+        <v>72.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for more Excel objects
Added support for:
Author
AllowEditRange, AllowEditRanges
CommentThreaded, CommentsThreaded
CustomProperty, CustomProperties
DataBarBorder
FileExportConverter, FileExportConverters
MultiThreadedCalculation
Outline
Protection
UserAccess, UserAccessList
</commit_message>
<xml_diff>
--- a/samples/XLSpy/sample.xlsx
+++ b/samples/XLSpy/sample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" backupFile="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7C6CB1-9134-4015-87ED-82419A0B1F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D391F4-5673-46DD-979E-1D8A0A831A64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a worksheet" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,21 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={B49ECDE9-7D16-488A-8870-578EAEE79461}</author>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{B49ECDE9-7D16-488A-8870-578EAEE79461}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This a new comment
+Reply:
+    Reply to a new comment</t>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -706,10 +717,10 @@
           <xdr:rowOff>106680</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>45720</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>236220</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>83820</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1373,13 +1384,24 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="L1" dT="2020-07-28T07:39:51.99" personId="{00000000-0000-0000-0000-000000000000}" id="{B49ECDE9-7D16-488A-8870-578EAEE79461}">
+    <text>This a new comment</text>
+  </threadedComment>
+  <threadedComment ref="L1" dT="2020-07-28T07:39:59.43" personId="{00000000-0000-0000-0000-000000000000}" id="{F64229CC-93F4-41FF-8747-5873137CEC3B}" parentId="{B49ECDE9-7D16-488A-8870-578EAEE79461}">
+    <text>Reply to a new comment</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,32 +1409,32 @@
     <col min="2" max="2" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>50</v>
       </c>
@@ -1443,10 +1465,10 @@
                 <xdr:rowOff>106680</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>45720</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>236220</xdr:colOff>
                 <xdr:row>16</xdr:row>
-                <xdr:rowOff>83820</xdr:rowOff>
+                <xdr:rowOff>45720</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1568,12 +1590,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
   </cols>

</xml_diff>